<commit_message>
docs(data): generate all genres evolution
</commit_message>
<xml_diff>
--- a/result/allGenresEvolution.xlsx
+++ b/result/allGenresEvolution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\Programing\Python\Fomalhaut\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53366CE-BED5-40E4-BB12-A633D91F7C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B545CC6-9473-4186-99E1-9C0265B93032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23490" yWindow="-1710" windowWidth="19125" windowHeight="10035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23490" yWindow="-1710" windowWidth="19125" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -134,10 +134,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -151,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -159,14 +167,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -506,53 +527,53 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1">
         <v>1995</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="1">
         <v>1996</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1">
         <v>1997</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="1">
         <v>1998</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="1">
         <v>1999</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="1">
         <v>2000</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="1">
         <v>2001</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="1">
         <v>2002</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="1">
         <v>2003</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="1">
         <v>2004</v>
       </c>
-      <c r="L1">
+      <c r="L1" s="1">
         <v>2005</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1884,5 +1905,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>